<commit_message>
fix unit tests for ubid
</commit_message>
<xml_diff>
--- a/seed/data_importer/tests/data/example-data-properties-small-changes.xlsx
+++ b/seed/data_importer/tests/data/example-data-properties-small-changes.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="29005"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nlong/working/seed/seed/data_importer/tests/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="51200" windowHeight="28260" tabRatio="151"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="16800" windowHeight="20480" tabRatio="151"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="114">
   <si>
     <t>521 Elm Street</t>
   </si>
@@ -316,6 +324,51 @@
   </si>
   <si>
     <t>Multistorys</t>
+  </si>
+  <si>
+    <t>UBID</t>
+  </si>
+  <si>
+    <t>https://ubid.org/65923-510</t>
+  </si>
+  <si>
+    <t>https://ubid.org/64942-1191</t>
+  </si>
+  <si>
+    <t>https://ubid.org/0093-2068</t>
+  </si>
+  <si>
+    <t>https://ubid.org/55316-267</t>
+  </si>
+  <si>
+    <t>https://ubid.org/62011-0243</t>
+  </si>
+  <si>
+    <t>https://ubid.org/49999-504</t>
+  </si>
+  <si>
+    <t>https://ubid.org/55289-460</t>
+  </si>
+  <si>
+    <t>https://ubid.org/60505-3404</t>
+  </si>
+  <si>
+    <t>https://ubid.org/55319-377</t>
+  </si>
+  <si>
+    <t>https://ubid.org/55505-167</t>
+  </si>
+  <si>
+    <t>https://ubid.org/61062-0007</t>
+  </si>
+  <si>
+    <t>https://ubid.org/0268-0851</t>
+  </si>
+  <si>
+    <t>https://ubid.org/68151-1305</t>
+  </si>
+  <si>
+    <t>https://ubid.org/54575-933</t>
   </si>
 </sst>
 </file>
@@ -943,32 +996,33 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T23"/>
+  <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32.33203125" style="12" customWidth="1"/>
     <col min="2" max="2" width="21.1640625" style="12" customWidth="1"/>
     <col min="3" max="3" width="20.5" style="12" customWidth="1"/>
     <col min="4" max="4" width="16.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" style="12" customWidth="1"/>
-    <col min="7" max="7" width="7.83203125" style="12" customWidth="1"/>
-    <col min="8" max="8" width="25.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.83203125" style="12" customWidth="1"/>
-    <col min="10" max="11" width="11.1640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.1640625" style="12" customWidth="1"/>
-    <col min="13" max="13" width="11.83203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="13.5" style="15" customWidth="1"/>
-    <col min="17" max="17" width="39" style="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.83203125" style="12"/>
+    <col min="5" max="5" width="25.5" style="12" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.6640625" style="12" customWidth="1"/>
+    <col min="8" max="8" width="7.83203125" style="12" customWidth="1"/>
+    <col min="9" max="9" width="25.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.83203125" style="12" customWidth="1"/>
+    <col min="11" max="12" width="11.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.1640625" style="12" customWidth="1"/>
+    <col min="14" max="14" width="11.83203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="13.5" style="15" customWidth="1"/>
+    <col min="18" max="18" width="39" style="12" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="8.83203125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" ht="12">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
         <v>86</v>
       </c>
@@ -982,53 +1036,56 @@
         <v>72</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="T1" s="4"/>
-    </row>
-    <row r="2" spans="1:20" s="5" customFormat="1">
+      <c r="U1" s="4"/>
+    </row>
+    <row r="2" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="5">
         <v>1</v>
       </c>
@@ -1036,54 +1093,57 @@
         <v>2264</v>
       </c>
       <c r="D2" s="6"/>
-      <c r="E2" s="6" t="s">
+      <c r="E2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H2" s="7">
+      <c r="I2" s="7">
         <v>1552813</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="J2" s="7">
+      <c r="K2" s="7">
         <v>91</v>
       </c>
-      <c r="K2" s="7">
+      <c r="L2" s="7">
         <v>125</v>
       </c>
-      <c r="L2" s="8">
+      <c r="M2" s="8">
         <v>42369</v>
       </c>
-      <c r="M2" s="9">
+      <c r="N2" s="9">
         <v>12555</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="O2" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="P2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="Q2" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="R2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="S2" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="S2" s="7">
+      <c r="T2" s="7">
         <v>1</v>
       </c>
-      <c r="T2" s="7"/>
-    </row>
-    <row r="3" spans="1:20" s="5" customFormat="1">
+      <c r="U2" s="7"/>
+    </row>
+    <row r="3" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="5">
         <v>4</v>
       </c>
@@ -1091,54 +1151,57 @@
         <v>1154623</v>
       </c>
       <c r="D3" s="6"/>
-      <c r="E3" s="6" t="s">
+      <c r="E3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="G3" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="H3" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H3" s="7">
+      <c r="I3" s="7">
         <v>11160509</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="J3" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="J3" s="7">
+      <c r="K3" s="7">
         <v>23</v>
       </c>
-      <c r="K3" s="7">
+      <c r="L3" s="7">
         <v>1202</v>
       </c>
-      <c r="L3" s="8">
+      <c r="M3" s="8">
         <v>42369</v>
       </c>
-      <c r="M3" s="9">
+      <c r="N3" s="9">
         <v>23543</v>
       </c>
-      <c r="N3" s="9" t="s">
+      <c r="O3" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="P3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="P3" s="9" t="s">
+      <c r="Q3" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="Q3" s="7" t="s">
+      <c r="R3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="R3" s="9" t="s">
+      <c r="S3" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="S3" s="7">
+      <c r="T3" s="7">
         <v>4</v>
       </c>
-      <c r="T3" s="7"/>
-    </row>
-    <row r="4" spans="1:20" s="5" customFormat="1">
+      <c r="U3" s="7"/>
+    </row>
+    <row r="4" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5">
         <v>6</v>
       </c>
@@ -1148,54 +1211,57 @@
       <c r="D4" s="5">
         <v>1311523</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="G4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="H4" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H4" s="7">
+      <c r="I4" s="7">
         <v>24651456</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="J4" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="J4" s="5">
+      <c r="K4" s="5">
         <v>32</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="L4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L4" s="8">
+      <c r="M4" s="8">
         <v>42369</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="N4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="N4" s="11" t="s">
+      <c r="O4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="5" t="s">
+      <c r="P4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="P4" s="11" t="s">
+      <c r="Q4" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="Q4" s="7" t="s">
+      <c r="R4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="R4" s="9" t="s">
+      <c r="S4" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="S4" s="7">
+      <c r="T4" s="7">
         <v>6</v>
       </c>
-      <c r="T4" s="12"/>
-    </row>
-    <row r="5" spans="1:20" s="5" customFormat="1">
+      <c r="U4" s="12"/>
+    </row>
+    <row r="5" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="5">
         <v>7</v>
       </c>
@@ -1205,54 +1271,57 @@
       <c r="D5" s="5">
         <v>1311523</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="G5" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="H5" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="7">
+      <c r="I5" s="7">
         <v>24651456</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="J5" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="J5" s="7">
+      <c r="K5" s="7">
         <v>12</v>
       </c>
-      <c r="K5" s="7">
+      <c r="L5" s="7">
         <v>219</v>
       </c>
-      <c r="L5" s="8">
+      <c r="M5" s="8">
         <v>42369</v>
       </c>
-      <c r="M5" s="13">
+      <c r="N5" s="13">
         <v>124523</v>
       </c>
-      <c r="N5" s="11" t="s">
+      <c r="O5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="O5" s="5" t="s">
+      <c r="P5" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="P5" s="11" t="s">
+      <c r="Q5" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="Q5" s="7" t="s">
+      <c r="R5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="R5" s="9" t="s">
+      <c r="S5" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="S5" s="7">
+      <c r="T5" s="7">
         <v>7</v>
       </c>
-      <c r="T5" s="12"/>
-    </row>
-    <row r="6" spans="1:20" s="5" customFormat="1">
+      <c r="U5" s="12"/>
+    </row>
+    <row r="6" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="5">
         <v>11</v>
       </c>
@@ -1262,54 +1331,57 @@
       <c r="D6" s="5">
         <v>1311523</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="G6" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="H6" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="7">
+      <c r="I6" s="7">
         <v>24651456</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="J6" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="J6" s="7">
+      <c r="K6" s="7">
         <v>43</v>
       </c>
-      <c r="K6" s="7">
+      <c r="L6" s="7">
         <v>84</v>
       </c>
-      <c r="L6" s="8">
+      <c r="M6" s="8">
         <v>42369</v>
       </c>
-      <c r="M6" s="13">
+      <c r="N6" s="13">
         <v>421351</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="O6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="O6" s="5" t="s">
+      <c r="P6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="P6" s="11" t="s">
+      <c r="Q6" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="Q6" s="7" t="s">
+      <c r="R6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="R6" s="9" t="s">
+      <c r="S6" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="S6" s="7">
+      <c r="T6" s="7">
         <v>8</v>
       </c>
-      <c r="T6" s="12"/>
-    </row>
-    <row r="7" spans="1:20">
+      <c r="U6" s="12"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="B7" s="5">
         <v>8</v>
@@ -1320,53 +1392,56 @@
       <c r="D7" s="5">
         <v>1311523</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="G7" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="H7" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H7" s="7">
+      <c r="I7" s="7">
         <v>24651456</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="J7" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="J7" s="7">
+      <c r="K7" s="7">
         <v>59</v>
       </c>
-      <c r="K7" s="7">
+      <c r="L7" s="7">
         <v>72</v>
       </c>
-      <c r="L7" s="8">
+      <c r="M7" s="8">
         <v>42369</v>
       </c>
-      <c r="M7" s="13">
+      <c r="N7" s="13">
         <v>1234</v>
       </c>
-      <c r="N7" s="11" t="s">
+      <c r="O7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="O7" s="5" t="s">
+      <c r="P7" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="P7" s="11" t="s">
+      <c r="Q7" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="Q7" s="7" t="s">
+      <c r="R7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="R7" s="9" t="s">
+      <c r="S7" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="S7" s="7">
+      <c r="T7" s="7">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
       <c r="B8" s="5">
         <v>9</v>
@@ -1377,53 +1452,56 @@
       <c r="D8" s="5">
         <v>1311523</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" t="s">
+        <v>106</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="G8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="H8" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="I8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="J8" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="J8" s="7">
+      <c r="K8" s="7">
         <v>34</v>
       </c>
-      <c r="K8" s="7">
+      <c r="L8" s="7">
         <v>45</v>
       </c>
-      <c r="L8" s="8">
+      <c r="M8" s="8">
         <v>42369</v>
       </c>
-      <c r="M8" s="13">
+      <c r="N8" s="13">
         <v>45324</v>
       </c>
-      <c r="N8" s="11" t="s">
+      <c r="O8" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="O8" s="5" t="s">
+      <c r="P8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="P8" s="11" t="s">
+      <c r="Q8" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="Q8" s="7" t="s">
+      <c r="R8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="R8" s="9" t="s">
+      <c r="S8" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="S8" s="7">
+      <c r="T8" s="7">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
       <c r="B9" s="5">
         <v>12</v>
@@ -1434,53 +1512,56 @@
       <c r="D9" s="5">
         <v>1311523</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="G9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="H9" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="I9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="J9" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="J9" s="5">
+      <c r="K9" s="5">
         <v>31</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="L9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L9" s="8">
+      <c r="M9" s="8">
         <v>42369</v>
       </c>
-      <c r="M9" s="13">
+      <c r="N9" s="13">
         <v>482215</v>
       </c>
-      <c r="N9" s="11" t="s">
+      <c r="O9" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="O9" s="5" t="s">
+      <c r="P9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="P9" s="11" t="s">
+      <c r="Q9" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="Q9" s="7" t="s">
+      <c r="R9" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="R9" s="9" t="s">
+      <c r="S9" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="S9" s="7">
+      <c r="T9" s="7">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
       <c r="B10" s="5">
         <v>2</v>
@@ -1489,54 +1570,57 @@
         <v>3020139</v>
       </c>
       <c r="D10" s="5"/>
-      <c r="E10" s="6" t="s">
+      <c r="E10" t="s">
+        <v>108</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="G10" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="H10" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H10" s="7">
+      <c r="I10" s="7">
         <v>11160509</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="J10" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J10" s="7">
+      <c r="K10" s="7">
         <v>1</v>
       </c>
-      <c r="K10" s="7">
+      <c r="L10" s="7">
         <v>652.29999999999995</v>
       </c>
-      <c r="L10" s="8">
+      <c r="M10" s="8">
         <v>42369</v>
       </c>
-      <c r="M10" s="9">
+      <c r="N10" s="9">
         <v>513852</v>
       </c>
-      <c r="N10" s="9" t="s">
+      <c r="O10" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="O10" s="5" t="s">
+      <c r="P10" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="P10" s="9" t="s">
+      <c r="Q10" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="Q10" s="7" t="s">
+      <c r="R10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="R10" s="9" t="s">
+      <c r="S10" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="S10" s="7">
+      <c r="T10" s="7">
         <v>2</v>
       </c>
-      <c r="T10" s="7"/>
-    </row>
-    <row r="11" spans="1:20">
+      <c r="U10" s="7"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
       <c r="B11" s="5">
         <v>3</v>
@@ -1545,54 +1629,57 @@
         <v>4828379</v>
       </c>
       <c r="D11" s="5"/>
-      <c r="E11" s="6" t="s">
+      <c r="E11" t="s">
+        <v>109</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="G11" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="H11" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H11" s="7">
+      <c r="I11" s="7">
         <v>11160509</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="J11" s="7" t="s">
         <v>88</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="K11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L11" s="8">
+      <c r="L11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M11" s="8">
         <v>42369</v>
       </c>
-      <c r="M11" s="9">
+      <c r="N11" s="9">
         <v>55121</v>
       </c>
-      <c r="N11" s="9" t="s">
+      <c r="O11" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="O11" s="5" t="s">
+      <c r="P11" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="P11" s="9" t="s">
+      <c r="Q11" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="Q11" s="7" t="s">
+      <c r="R11" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="R11" s="9" t="s">
+      <c r="S11" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="S11" s="7">
+      <c r="T11" s="7">
         <v>3</v>
       </c>
-      <c r="T11" s="7"/>
-    </row>
-    <row r="12" spans="1:20">
+      <c r="U11" s="7"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
       <c r="B12" s="5">
         <v>5</v>
@@ -1601,107 +1688,113 @@
         <v>5233255</v>
       </c>
       <c r="D12" s="6"/>
-      <c r="E12" s="6" t="s">
+      <c r="E12" t="s">
+        <v>110</v>
+      </c>
+      <c r="F12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="G12" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="H12" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="I12" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="I12" s="7" t="s">
+      <c r="J12" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="J12" s="7">
+      <c r="K12" s="7">
         <v>55</v>
       </c>
-      <c r="K12" s="7">
+      <c r="L12" s="7">
         <v>1358</v>
       </c>
-      <c r="L12" s="8">
+      <c r="M12" s="8">
         <v>42369</v>
       </c>
-      <c r="M12" s="9">
+      <c r="N12" s="9">
         <v>200000</v>
       </c>
-      <c r="N12" s="9" t="s">
+      <c r="O12" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="O12" s="5" t="s">
+      <c r="P12" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="P12" s="9" t="s">
+      <c r="Q12" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="Q12" s="7" t="s">
+      <c r="R12" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="R12" s="9" t="s">
+      <c r="S12" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="S12" s="7">
+      <c r="T12" s="7">
         <v>5</v>
       </c>
-      <c r="T12" s="7"/>
-    </row>
-    <row r="13" spans="1:20">
+      <c r="U12" s="7"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B13" s="5">
         <v>10</v>
       </c>
       <c r="C13" s="6">
         <v>6798215</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" t="s">
+        <v>111</v>
+      </c>
+      <c r="F13" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="G13" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="H13" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H13" s="16">
+      <c r="I13" s="16">
         <v>13334485</v>
       </c>
-      <c r="I13" s="7" t="s">
+      <c r="J13" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="J13" s="7">
+      <c r="K13" s="7">
         <v>88</v>
       </c>
-      <c r="K13" s="7">
+      <c r="L13" s="7">
         <v>942</v>
       </c>
-      <c r="L13" s="8">
+      <c r="M13" s="8">
         <v>42369</v>
       </c>
-      <c r="M13" s="14">
+      <c r="N13" s="14">
         <v>24523</v>
       </c>
-      <c r="N13" s="15" t="s">
+      <c r="O13" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="O13" s="12" t="s">
+      <c r="P13" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="P13" s="15" t="s">
+      <c r="Q13" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="Q13" s="7" t="s">
+      <c r="R13" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="R13" s="9" t="s">
+      <c r="S13" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="S13" s="7">
+      <c r="T13" s="7">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="17"/>
       <c r="B14" s="17">
         <v>13</v>
@@ -1710,54 +1803,57 @@
         <v>481516</v>
       </c>
       <c r="D14" s="17"/>
-      <c r="E14" s="18" t="s">
+      <c r="E14" t="s">
+        <v>112</v>
+      </c>
+      <c r="F14" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="F14" s="18" t="s">
+      <c r="G14" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="G14" s="18" t="s">
+      <c r="H14" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="H14" s="17">
+      <c r="I14" s="17">
         <v>1234</v>
       </c>
-      <c r="I14" s="18" t="s">
+      <c r="J14" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="J14" s="18">
+      <c r="K14" s="18">
         <v>34</v>
       </c>
-      <c r="K14" s="18">
+      <c r="L14" s="18">
         <v>45</v>
       </c>
-      <c r="L14" s="19">
+      <c r="M14" s="19">
         <v>42369</v>
       </c>
-      <c r="M14" s="20">
+      <c r="N14" s="20">
         <v>45324</v>
       </c>
-      <c r="N14" s="21" t="s">
+      <c r="O14" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="O14" s="17" t="s">
+      <c r="P14" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="P14" s="21" t="s">
+      <c r="Q14" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="Q14" s="17" t="s">
+      <c r="R14" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="R14" s="22" t="s">
+      <c r="S14" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="S14" s="17">
+      <c r="T14" s="17">
         <v>10</v>
       </c>
-      <c r="T14" s="17"/>
-    </row>
-    <row r="15" spans="1:20">
+      <c r="U14" s="17"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="17"/>
       <c r="B15" s="17">
         <v>13</v>
@@ -1766,79 +1862,92 @@
         <v>2342</v>
       </c>
       <c r="D15" s="17"/>
-      <c r="E15" s="18" t="s">
+      <c r="E15" t="s">
+        <v>113</v>
+      </c>
+      <c r="F15" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="F15" s="18" t="s">
+      <c r="G15" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="G15" s="18" t="s">
+      <c r="H15" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="H15" s="17">
+      <c r="I15" s="17">
         <v>4321</v>
       </c>
-      <c r="I15" s="18" t="s">
+      <c r="J15" s="18" t="s">
         <v>22</v>
-      </c>
-      <c r="J15" s="17" t="s">
-        <v>24</v>
       </c>
       <c r="K15" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="L15" s="19">
+      <c r="L15" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="M15" s="19">
         <v>42369</v>
       </c>
-      <c r="M15" s="20">
+      <c r="N15" s="20">
         <v>125000</v>
       </c>
-      <c r="N15" s="21" t="s">
+      <c r="O15" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="O15" s="17" t="s">
+      <c r="P15" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="P15" s="21" t="s">
+      <c r="Q15" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="Q15" s="17" t="s">
+      <c r="R15" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="R15" s="22" t="s">
+      <c r="S15" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="S15" s="17">
+      <c r="T15" s="17">
         <v>11</v>
       </c>
-      <c r="T15" s="17"/>
-    </row>
-    <row r="17" spans="8:8">
-      <c r="H17" s="7"/>
-    </row>
-    <row r="18" spans="8:8">
-      <c r="H18" s="7"/>
-    </row>
-    <row r="19" spans="8:8">
-      <c r="H19" s="7"/>
-    </row>
-    <row r="20" spans="8:8">
-      <c r="H20" s="7"/>
-    </row>
-    <row r="21" spans="8:8">
-      <c r="H21" s="7"/>
-    </row>
-    <row r="22" spans="8:8">
-      <c r="H22" s="7"/>
-    </row>
-    <row r="23" spans="8:8">
-      <c r="H23" s="5"/>
+      <c r="U15" s="17"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="E16"/>
+    </row>
+    <row r="17" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E17"/>
+      <c r="I17" s="7"/>
+    </row>
+    <row r="18" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E18"/>
+      <c r="I18" s="7"/>
+    </row>
+    <row r="19" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E19"/>
+      <c r="I19" s="7"/>
+    </row>
+    <row r="20" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E20"/>
+      <c r="I20" s="7"/>
+    </row>
+    <row r="21" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E21"/>
+      <c r="I21" s="7"/>
+    </row>
+    <row r="22" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E22"/>
+      <c r="I22" s="7"/>
+    </row>
+    <row r="23" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E23"/>
+      <c r="I23" s="5"/>
     </row>
   </sheetData>
   <sortState ref="A2:T13">
     <sortCondition ref="B2:B13"/>
   </sortState>
-  <conditionalFormatting sqref="C2:E2 E3:E4 C9 C11 C5:E6 C7 E7:E13">
+  <conditionalFormatting sqref="C2:D2 C9 C11 C5:D6 C7 F2:F13">
     <cfRule type="duplicateValues" dxfId="2" priority="97"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8 C10 C12">
@@ -1850,10 +1959,5 @@
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
highlight the differences in the small changes file
</commit_message>
<xml_diff>
--- a/seed/data_importer/tests/data/example-data-properties-small-changes.xlsx
+++ b/seed/data_importer/tests/data/example-data-properties-small-changes.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="29005"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10910"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nlong/working/seed/seed/data_importer/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A05BD659-432C-8540-B485-C0C8407F7E49}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="28260" tabRatio="151"/>
+    <workbookView xWindow="0" yWindow="14580" windowWidth="51200" windowHeight="14220" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -374,7 +375,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -438,12 +439,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -539,7 +546,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -580,6 +587,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="82">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -701,6 +714,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -992,14 +1008,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E15"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1025,7 +1041,7 @@
     <col min="21" max="16384" width="8.83203125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
         <v>86</v>
       </c>
@@ -1111,10 +1127,10 @@
       <c r="I2" s="7">
         <v>1552813</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="K2" s="7">
+      <c r="K2" s="24">
         <v>91</v>
       </c>
       <c r="L2" s="7">
@@ -1169,10 +1185,10 @@
       <c r="I3" s="7">
         <v>11160509</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="24">
         <v>23</v>
       </c>
       <c r="L3" s="7">
@@ -1229,10 +1245,10 @@
       <c r="I4" s="7">
         <v>24651456</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="25">
         <v>32</v>
       </c>
       <c r="L4" s="5" t="s">
@@ -1289,10 +1305,10 @@
       <c r="I5" s="7">
         <v>24651456</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="24">
         <v>12</v>
       </c>
       <c r="L5" s="7">
@@ -1349,7 +1365,7 @@
       <c r="I6" s="7">
         <v>24651456</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="24" t="s">
         <v>91</v>
       </c>
       <c r="K6" s="7">
@@ -1410,7 +1426,7 @@
       <c r="I7" s="7">
         <v>24651456</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="J7" s="24" t="s">
         <v>92</v>
       </c>
       <c r="K7" s="7">
@@ -1470,7 +1486,7 @@
       <c r="I8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="J8" s="24" t="s">
         <v>93</v>
       </c>
       <c r="K8" s="7">
@@ -1530,10 +1546,10 @@
       <c r="I9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J9" s="7" t="s">
+      <c r="J9" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="K9" s="5">
+      <c r="K9" s="25">
         <v>31</v>
       </c>
       <c r="L9" s="5" t="s">
@@ -1647,7 +1663,7 @@
       <c r="I11" s="7">
         <v>11160509</v>
       </c>
-      <c r="J11" s="7" t="s">
+      <c r="J11" s="24" t="s">
         <v>88</v>
       </c>
       <c r="K11" s="5" t="s">
@@ -1706,7 +1722,7 @@
       <c r="I12" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="J12" s="7" t="s">
+      <c r="J12" s="24" t="s">
         <v>96</v>
       </c>
       <c r="K12" s="7">
@@ -1763,7 +1779,7 @@
       <c r="I13" s="16">
         <v>13334485</v>
       </c>
-      <c r="J13" s="7" t="s">
+      <c r="J13" s="24" t="s">
         <v>98</v>
       </c>
       <c r="K13" s="7">
@@ -1797,7 +1813,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="17"/>
       <c r="B14" s="17">
         <v>13</v>
@@ -1821,7 +1837,7 @@
       <c r="I14" s="17">
         <v>1234</v>
       </c>
-      <c r="J14" s="18" t="s">
+      <c r="J14" s="26" t="s">
         <v>97</v>
       </c>
       <c r="K14" s="18">
@@ -1856,7 +1872,7 @@
       </c>
       <c r="U14" s="17"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="17"/>
       <c r="B15" s="17">
         <v>13</v>
@@ -1892,7 +1908,7 @@
       <c r="M15" s="19">
         <v>42369</v>
       </c>
-      <c r="N15" s="20">
+      <c r="N15" s="27">
         <v>125000</v>
       </c>
       <c r="O15" s="21" t="s">
@@ -1950,7 +1966,7 @@
   <sortState ref="A2:T13">
     <sortCondition ref="B2:B13"/>
   </sortState>
-  <conditionalFormatting sqref="C2:D2 C9 C11 C5:D6 C7 F2:F13">
+  <conditionalFormatting sqref="C2:D2 C9 C11 C6:D6 C7 F2:F13 C5">
     <cfRule type="duplicateValues" dxfId="2" priority="97"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8 C10 C12">

</xml_diff>

<commit_message>
more string literal cleanup
</commit_message>
<xml_diff>
--- a/seed/data_importer/tests/data/example-data-properties-small-changes.xlsx
+++ b/seed/data_importer/tests/data/example-data-properties-small-changes.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="29005"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10910"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nlong/working/seed/seed/data_importer/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A05BD659-432C-8540-B485-C0C8407F7E49}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="28260" tabRatio="151"/>
+    <workbookView xWindow="0" yWindow="14580" windowWidth="51200" windowHeight="14220" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -374,7 +375,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -438,12 +439,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -539,7 +546,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -580,6 +587,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="82">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -701,6 +714,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -992,14 +1008,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E15"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1025,7 +1041,7 @@
     <col min="21" max="16384" width="8.83203125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
         <v>86</v>
       </c>
@@ -1111,10 +1127,10 @@
       <c r="I2" s="7">
         <v>1552813</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="K2" s="7">
+      <c r="K2" s="24">
         <v>91</v>
       </c>
       <c r="L2" s="7">
@@ -1169,10 +1185,10 @@
       <c r="I3" s="7">
         <v>11160509</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="24">
         <v>23</v>
       </c>
       <c r="L3" s="7">
@@ -1229,10 +1245,10 @@
       <c r="I4" s="7">
         <v>24651456</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="25">
         <v>32</v>
       </c>
       <c r="L4" s="5" t="s">
@@ -1289,10 +1305,10 @@
       <c r="I5" s="7">
         <v>24651456</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="24">
         <v>12</v>
       </c>
       <c r="L5" s="7">
@@ -1349,7 +1365,7 @@
       <c r="I6" s="7">
         <v>24651456</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="24" t="s">
         <v>91</v>
       </c>
       <c r="K6" s="7">
@@ -1410,7 +1426,7 @@
       <c r="I7" s="7">
         <v>24651456</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="J7" s="24" t="s">
         <v>92</v>
       </c>
       <c r="K7" s="7">
@@ -1470,7 +1486,7 @@
       <c r="I8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="J8" s="24" t="s">
         <v>93</v>
       </c>
       <c r="K8" s="7">
@@ -1530,10 +1546,10 @@
       <c r="I9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J9" s="7" t="s">
+      <c r="J9" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="K9" s="5">
+      <c r="K9" s="25">
         <v>31</v>
       </c>
       <c r="L9" s="5" t="s">
@@ -1647,7 +1663,7 @@
       <c r="I11" s="7">
         <v>11160509</v>
       </c>
-      <c r="J11" s="7" t="s">
+      <c r="J11" s="24" t="s">
         <v>88</v>
       </c>
       <c r="K11" s="5" t="s">
@@ -1706,7 +1722,7 @@
       <c r="I12" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="J12" s="7" t="s">
+      <c r="J12" s="24" t="s">
         <v>96</v>
       </c>
       <c r="K12" s="7">
@@ -1763,7 +1779,7 @@
       <c r="I13" s="16">
         <v>13334485</v>
       </c>
-      <c r="J13" s="7" t="s">
+      <c r="J13" s="24" t="s">
         <v>98</v>
       </c>
       <c r="K13" s="7">
@@ -1797,7 +1813,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="17"/>
       <c r="B14" s="17">
         <v>13</v>
@@ -1821,7 +1837,7 @@
       <c r="I14" s="17">
         <v>1234</v>
       </c>
-      <c r="J14" s="18" t="s">
+      <c r="J14" s="26" t="s">
         <v>97</v>
       </c>
       <c r="K14" s="18">
@@ -1856,7 +1872,7 @@
       </c>
       <c r="U14" s="17"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="17"/>
       <c r="B15" s="17">
         <v>13</v>
@@ -1892,7 +1908,7 @@
       <c r="M15" s="19">
         <v>42369</v>
       </c>
-      <c r="N15" s="20">
+      <c r="N15" s="27">
         <v>125000</v>
       </c>
       <c r="O15" s="21" t="s">
@@ -1950,7 +1966,7 @@
   <sortState ref="A2:T13">
     <sortCondition ref="B2:B13"/>
   </sortState>
-  <conditionalFormatting sqref="C2:D2 C9 C11 C5:D6 C7 F2:F13">
+  <conditionalFormatting sqref="C2:D2 C9 C11 C6:D6 C7 F2:F13 C5">
     <cfRule type="duplicateValues" dxfId="2" priority="97"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8 C10 C12">

</xml_diff>